<commit_message>
building xpath to select hotel
</commit_message>
<xml_diff>
--- a/Data Files/data2_bookings_KatalonTests.xlsx
+++ b/Data Files/data2_bookings_KatalonTests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres.Jaramillo\git\bookit-bookingtests-katalon\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E12C10B-9E32-4618-B64B-242C62221AA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BD42D4-F56D-4CF6-BBD7-6D202EA7CB38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>yrIni</t>
   </si>
@@ -83,6 +83,33 @@
   </si>
   <si>
     <t>1,2</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Cheese City Per Person, IL, US</t>
+  </si>
+  <si>
+    <t>hotelname</t>
+  </si>
+  <si>
+    <t>Cheese Automation Testing Resort</t>
+  </si>
+  <si>
+    <t>Chocolate Cheesecake Beach</t>
+  </si>
+  <si>
+    <t>Cheese Cake Island Hotel</t>
   </si>
 </sst>
 </file>
@@ -455,161 +482,185 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>2</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
       </c>
       <c r="H5" s="3">
         <v>1</v>
@@ -618,7 +669,13 @@
         <v>1</v>
       </c>
       <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
         <v>5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>